<commit_message>
validatie.ipynb werkt nu vanaf de omgezette karteringen
</commit_message>
<xml_diff>
--- a/data/validationinfo.xlsx
+++ b/data/validationinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD70466-4A65-478B-9A27-3561E9A711B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1999D32F-9114-43C6-874D-51094A847027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>provincie</t>
   </si>
@@ -60,9 +60,6 @@
     <t>SBB ZWK 2010 0815_Trimunt_2010</t>
   </si>
   <si>
-    <t>SGL Zuidlaardermeer 2019</t>
-  </si>
-  <si>
     <t>./Habitatkarteringen/Habitattypekaarten Gr/NaamGebied_Westerwolde.gpkg</t>
   </si>
   <si>
@@ -165,13 +162,46 @@
     <t>Habtype</t>
   </si>
   <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>naam_in_overzicht_vegkart</t>
-  </si>
-  <si>
     <t>naam_in_overzicht_habkart</t>
+  </si>
+  <si>
+    <t>./GR/SBB Westerwolde 2020/GISbestanden/vlakken.shp</t>
+  </si>
+  <si>
+    <t>./GR/SBB ZWK 2010/0814_Tussen de Gasten 2010/ZWK0814_2010.shp</t>
+  </si>
+  <si>
+    <t>./GR/SBB ZWK 2010/0815_Trimunt_2010/vlakken.shp</t>
+  </si>
+  <si>
+    <t>./GR/NM vegetatiekartering RuitenAa2020 edited/vegkart_RuitenA_2020/vegkart_RuitenA_2020.shp</t>
+  </si>
+  <si>
+    <t>./GR/SGL Zuidlaardermeer 2019/kartering zuidlaardermeer 2019 definitief/GIS-bestanden Zuidlaardermeer 2019/GIS_Vlakken_zuidlaardermeer_2019/vlakken.shp</t>
+  </si>
+  <si>
+    <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatiekartering Leekstermeer2021/GIS bestanden Onlanden 2021/Vegetatiekartering_Leekstermeer2021.shp</t>
+  </si>
+  <si>
+    <t>./GR/SBB Lauwersmeer 2015/vlakken.shp</t>
+  </si>
+  <si>
+    <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatie- en plantensoortenkartering Hunzedal concept/gis/Vegetatiekartering_Hunzedal2021.shp</t>
+  </si>
+  <si>
+    <t>path_pred</t>
+  </si>
+  <si>
+    <t>path_true</t>
+  </si>
+  <si>
+    <t>werkt_nu</t>
+  </si>
+  <si>
+    <t>reden dat hij niet werkt</t>
+  </si>
+  <si>
+    <t>De kartering die wij hebben heebt geen unieke ElmID kolom; dus kunnen vlakken niet met zekerheid aan vegetatietypen gekoppeld worden</t>
   </si>
 </sst>
 </file>
@@ -195,18 +225,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,10 +245,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,32 +541,40 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="81.7109375" customWidth="1"/>
     <col min="5" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="12" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="165.28515625" customWidth="1"/>
+    <col min="9" max="12" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -552,32 +583,38 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -586,15 +623,18 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -603,49 +643,61 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -654,129 +706,162 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -784,21 +869,27 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -806,29 +897,38 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support for non-groningen validation
</commit_message>
<xml_diff>
--- a/data/validationinfo.xlsx
+++ b/data/validationinfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1999D32F-9114-43C6-874D-51094A847027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14474C1B-C1F4-436B-B0FF-96DDE1102FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21540" yWindow="1005" windowWidth="37080" windowHeight="16830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
   <si>
     <t>provincie</t>
   </si>
@@ -123,9 +123,6 @@
     <t>SBB1034_Dwingelderveld2017</t>
   </si>
   <si>
-    <t>in vegetatiekartering</t>
-  </si>
-  <si>
     <t>Drouwenerzand_2020</t>
   </si>
   <si>
@@ -153,15 +150,6 @@
     <t>BosGroep_SNLMonitoring_2014</t>
   </si>
   <si>
-    <t>percentage_cols</t>
-  </si>
-  <si>
-    <t>habtype_cols</t>
-  </si>
-  <si>
-    <t>Habtype</t>
-  </si>
-  <si>
     <t>naam_in_overzicht_habkart</t>
   </si>
   <si>
@@ -201,7 +189,94 @@
     <t>reden dat hij niet werkt</t>
   </si>
   <si>
-    <t>De kartering die wij hebben heebt geen unieke ElmID kolom; dus kunnen vlakken niet met zekerheid aan vegetatietypen gekoppeld worden</t>
+    <t>habtype_cols_regex</t>
+  </si>
+  <si>
+    <t>percentage_cols_regex</t>
+  </si>
+  <si>
+    <t>Habtype\d+</t>
+  </si>
+  <si>
+    <t>habitatType\dCode</t>
+  </si>
+  <si>
+    <t>bedekkingsPercentage\d</t>
+  </si>
+  <si>
+    <t>Habtype\d</t>
+  </si>
+  <si>
+    <t>Perc\d</t>
+  </si>
+  <si>
+    <t>habitatType\d</t>
+  </si>
+  <si>
+    <t>HABTYPE1</t>
+  </si>
+  <si>
+    <t>PERC1</t>
+  </si>
+  <si>
+    <t>./Habitatkarteringen/Habitattypekaarten Dr/uit vegetatiekartering/PRV_Witterdiep2021/PRV_Witterdiep2021.shp</t>
+  </si>
+  <si>
+    <t>Heeft SBB codes in een gestructureerde omzettabel - deze is nog niet omgezet, dus we hebben nog geen omgezette vegetatiekartering</t>
+  </si>
+  <si>
+    <t>De kartering die wij hebben heeft geen unieke ElmID kolom; dus kunnen vlakken niet met zekerheid aan vegetatietypen gekoppeld worden</t>
+  </si>
+  <si>
+    <t>./Habitatkarteringen/Habitattypekaarten Dr/Mantingerzand/32_T1_V4_20230914.gdb</t>
+  </si>
+  <si>
+    <t>./FR/Duinen_Schiermonnikoog/Schiermonnikoog_2015/gis/vlakken.shp</t>
+  </si>
+  <si>
+    <t>./DR Extra/NM_Mantingerveld2015/NM_2015_Mantingerbos.shp</t>
+  </si>
+  <si>
+    <t>./DR/SBB1034_Dwingelderveld2017/SBB1034_Dwingelderveld2017.shp</t>
+  </si>
+  <si>
+    <t>./DR Extra/2020_Drouwenerzand/HDL_Drouwenerzand_2020.shp</t>
+  </si>
+  <si>
+    <t>./DR/NM_Fochteloerveen2013_14/NM_Fochteloerveen2013_14.shp</t>
+  </si>
+  <si>
+    <t>./DR/NM_SBB_Fochteloerveen_randen2016/NM_SBB_Fochteloerveen_randen2016.shp</t>
+  </si>
+  <si>
+    <t>./DR/SBB0816_Norg2010/SBB0816Norg2010.shp</t>
+  </si>
+  <si>
+    <t>./DR Extra/definitief Fochteloo_Norg2020/GISbestanden_Fochteloo_Norg2020/VlakkenVegetatiekarteringFochteloo_210331/NM_Fovhteloerveen_Norg2020.shp</t>
+  </si>
+  <si>
+    <t>./DR/BG_Drenthe2014/Bosgroep_SNLmonitoring2014.gdb/Bosgroep_SNLmonitoring2014.shp</t>
+  </si>
+  <si>
+    <t>./DR Extra/NM_DCR2013/NM_Fochteloerveen_DCR2013.shp</t>
+  </si>
+  <si>
+    <t>./DR/PRV_Witterdiep2021/PRV_Witterdiep2021.shp</t>
+  </si>
+  <si>
+    <t>./FR/Duinen_Vlieland/Vegetatiekartering 2013/Vlieland_vlakken_VegType.shp</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t>./Habitatkarteringen/Habitattypekaarten Dr/Drouwenerzand/26_T1_V3_20231205.gdb</t>
+  </si>
+  <si>
+    <t>Staat niet in overzicht_vegetatiekarteringen, dus zetten we niet om</t>
   </si>
 </sst>
 </file>
@@ -528,53 +603,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="81.7109375" customWidth="1"/>
-    <col min="5" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="165.28515625" customWidth="1"/>
-    <col min="9" max="12" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="70.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="7" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="165.28515625" customWidth="1"/>
+    <col min="10" max="13" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>42</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -586,15 +665,15 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -606,15 +685,15 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>44</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -626,15 +705,15 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -646,18 +725,18 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="b">
+        <v>56</v>
+      </c>
+      <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -669,15 +748,15 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -689,15 +768,15 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -709,15 +788,15 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -729,13 +808,16 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -745,11 +827,20 @@
       <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -759,11 +850,17 @@
       <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -773,11 +870,23 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="G12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -787,11 +896,20 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -801,67 +919,124 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -869,27 +1044,51 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -897,37 +1096,70 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" t="b">
+        <v>64</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>